<commit_message>
update grading template and include HighRoll starter code
</commit_message>
<xml_diff>
--- a/spring20/assignment03/Grading Template.xlsx
+++ b/spring20/assignment03/Grading Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aavol\Documents\LMU\CMSI 186 - Spring 2020\Github\Volosin\cmsi186\spring20\assignment03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8885541E-5569-4976-8750-518AA423C9E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770FD854-BCF7-4FF8-A082-3F18C7DAEBC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" xr2:uid="{63A3425B-6033-479B-8BF1-9D375DE2499F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>#</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>option 8 display menu works (do not display menu every time a user inputs a menu option</t>
+  </si>
+  <si>
+    <t>program handles invalid number of arguments</t>
+  </si>
+  <si>
+    <t>parsing args to ints is in a try catch</t>
   </si>
 </sst>
 </file>
@@ -293,6 +299,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -305,7 +312,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A814EA-F008-428D-8D17-C9F98DC7D045}">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -658,7 +664,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="17" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="4">
@@ -673,7 +679,7 @@
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="16"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="4">
         <v>2</v>
       </c>
@@ -686,7 +692,7 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="16"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="4">
         <v>3</v>
       </c>
@@ -699,7 +705,7 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B7" s="16"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="4">
         <v>4</v>
       </c>
@@ -712,7 +718,7 @@
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="16"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="4">
         <v>5</v>
       </c>
@@ -725,7 +731,7 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="16"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="4">
         <v>6</v>
       </c>
@@ -738,7 +744,7 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B10" s="16"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="4">
         <v>7</v>
       </c>
@@ -751,7 +757,7 @@
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="16"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="4">
         <v>8</v>
       </c>
@@ -764,7 +770,7 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="16"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="4">
         <v>9</v>
       </c>
@@ -810,7 +816,7 @@
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="18" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="8">
@@ -825,7 +831,7 @@
       <c r="F16" s="9"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B17" s="16"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="4">
         <v>2</v>
       </c>
@@ -838,7 +844,7 @@
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B18" s="16"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="4">
         <v>3</v>
       </c>
@@ -851,7 +857,7 @@
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B19" s="16"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="4">
         <v>4</v>
       </c>
@@ -864,7 +870,7 @@
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="16"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="4">
         <v>5</v>
       </c>
@@ -877,7 +883,7 @@
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B21" s="16"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="4">
         <v>6</v>
       </c>
@@ -890,7 +896,7 @@
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B22" s="16"/>
+      <c r="B22" s="17"/>
       <c r="C22" s="4">
         <v>7</v>
       </c>
@@ -903,7 +909,7 @@
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B23" s="16"/>
+      <c r="B23" s="17"/>
       <c r="C23" s="4">
         <v>8</v>
       </c>
@@ -916,7 +922,7 @@
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B24" s="16"/>
+      <c r="B24" s="17"/>
       <c r="C24" s="4">
         <v>9</v>
       </c>
@@ -929,7 +935,7 @@
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B25" s="16"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="4">
         <v>10</v>
       </c>
@@ -942,7 +948,7 @@
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B26" s="16"/>
+      <c r="B26" s="17"/>
       <c r="C26" s="4">
         <v>11</v>
       </c>
@@ -955,7 +961,7 @@
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B27" s="16"/>
+      <c r="B27" s="17"/>
       <c r="C27" s="4">
         <v>12</v>
       </c>
@@ -968,7 +974,7 @@
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B28" s="16"/>
+      <c r="B28" s="17"/>
       <c r="C28" s="4">
         <v>13</v>
       </c>
@@ -981,7 +987,7 @@
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B29" s="16"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="4">
         <v>14</v>
       </c>
@@ -994,7 +1000,7 @@
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B30" s="16"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="4">
         <v>15</v>
       </c>
@@ -1007,21 +1013,21 @@
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B31" s="16"/>
+      <c r="B31" s="17"/>
       <c r="C31" s="4"/>
       <c r="D31" s="7"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B32" s="16"/>
+      <c r="B32" s="17"/>
       <c r="C32" s="4"/>
       <c r="D32" s="5"/>
       <c r="E32" s="6"/>
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="12">
@@ -1036,7 +1042,7 @@
       <c r="F33" s="9"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B34" s="16"/>
+      <c r="B34" s="17"/>
       <c r="C34" s="11">
         <v>2</v>
       </c>
@@ -1049,227 +1055,249 @@
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B35" s="16"/>
+      <c r="B35" s="17"/>
       <c r="C35" s="11">
+        <v>4</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" s="7"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B36" s="17"/>
+      <c r="C36" s="11">
+        <v>5</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="7"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B37" s="17"/>
+      <c r="C37" s="11">
+        <v>6</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="5">
+        <v>6</v>
+      </c>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B38" s="17"/>
+      <c r="C38" s="11">
+        <v>7</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38" s="5">
+        <v>4</v>
+      </c>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B39" s="17"/>
+      <c r="C39" s="11">
+        <v>8</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="5">
+        <v>4</v>
+      </c>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B40" s="17"/>
+      <c r="C40" s="11">
+        <v>9</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="5">
+        <v>4</v>
+      </c>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B41" s="17"/>
+      <c r="C41" s="11">
+        <v>10</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="5">
+        <v>4</v>
+      </c>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B42" s="17"/>
+      <c r="C42" s="11">
+        <v>11</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="5">
+        <v>4</v>
+      </c>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B43" s="17"/>
+      <c r="C43" s="11">
+        <v>12</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="7">
+        <v>4</v>
+      </c>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B44" s="17"/>
+      <c r="C44" s="11">
+        <v>13</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="7">
+        <v>5</v>
+      </c>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B45" s="17"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B46" s="17"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B47" s="19"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="6">
+        <v>1</v>
+      </c>
+      <c r="F47" s="6"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B48" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="12">
+        <v>1</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="9">
+        <v>1</v>
+      </c>
+      <c r="F48" s="9"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B49" s="17"/>
+      <c r="C49" s="11">
+        <v>2</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" s="5">
+        <v>1</v>
+      </c>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B50" s="17"/>
+      <c r="C50" s="11">
         <v>3</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D50" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="5">
+        <v>3</v>
+      </c>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B51" s="19"/>
+      <c r="C51" s="14">
+        <v>4</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" s="6">
         <v>10</v>
       </c>
-      <c r="E35" s="5">
-        <v>6</v>
-      </c>
-      <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B36" s="16"/>
-      <c r="C36" s="11">
-        <v>4</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E36" s="5">
-        <v>4</v>
-      </c>
-      <c r="F36" s="5"/>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B37" s="16"/>
-      <c r="C37" s="11">
-        <v>5</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="5">
-        <v>4</v>
-      </c>
-      <c r="F37" s="5"/>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B38" s="16"/>
-      <c r="C38" s="11">
-        <v>6</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E38" s="5">
-        <v>4</v>
-      </c>
-      <c r="F38" s="5"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B39" s="16"/>
-      <c r="C39" s="11">
-        <v>7</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" s="5">
-        <v>4</v>
-      </c>
-      <c r="F39" s="5"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B40" s="16"/>
-      <c r="C40" s="11">
-        <v>8</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" s="5">
-        <v>4</v>
-      </c>
-      <c r="F40" s="5"/>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B41" s="16"/>
-      <c r="C41" s="11">
-        <v>9</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E41" s="7">
-        <v>4</v>
-      </c>
-      <c r="F41" s="5"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B42" s="16"/>
-      <c r="C42" s="11">
-        <v>10</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E42" s="7">
-        <v>5</v>
-      </c>
-      <c r="F42" s="5"/>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B43" s="16"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B44" s="16"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B45" s="18"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="6">
-        <v>1</v>
-      </c>
-      <c r="F45" s="6"/>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B46" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C46" s="12">
-        <v>1</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E46" s="9">
-        <v>1</v>
-      </c>
-      <c r="F46" s="9"/>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B47" s="16"/>
-      <c r="C47" s="11">
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B52" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52" s="12">
+        <v>1</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E52" s="9">
         <v>2</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E47" s="5">
-        <v>1</v>
-      </c>
-      <c r="F47" s="5"/>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B48" s="16"/>
-      <c r="C48" s="11">
-        <v>3</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E48" s="5">
-        <v>3</v>
-      </c>
-      <c r="F48" s="5"/>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B49" s="18"/>
-      <c r="C49" s="14">
-        <v>4</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E49" s="6">
-        <v>10</v>
-      </c>
-      <c r="F49" s="6"/>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B50" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C50" s="12">
-        <v>1</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E50" s="9">
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B53" s="17"/>
+      <c r="C53" s="11">
         <v>2</v>
       </c>
-      <c r="F50" s="5"/>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B51" s="16"/>
-      <c r="C51" s="11">
+      <c r="D53" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E53" s="7">
         <v>2</v>
       </c>
-      <c r="D51" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E51" s="7">
-        <v>2</v>
-      </c>
-      <c r="F51" s="5"/>
-    </row>
-    <row r="52" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="19"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="5"/>
-    </row>
-    <row r="53" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D53" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E53">
-        <f>SUM(E4:E49)</f>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B54" s="20"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="D55" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E55">
+        <f>SUM(E4:E51)</f>
         <v>123</v>
       </c>
     </row>
@@ -1277,9 +1305,9 @@
   <mergeCells count="5">
     <mergeCell ref="B4:B12"/>
     <mergeCell ref="B16:B32"/>
-    <mergeCell ref="B33:B45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B33:B47"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="B52:B54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update grading template, update highroll starter code
</commit_message>
<xml_diff>
--- a/spring20/assignment03/Grading Template.xlsx
+++ b/spring20/assignment03/Grading Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aavol\Documents\LMU\CMSI 186 - Spring 2020\Github\Volosin\cmsi186\spring20\assignment03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770FD854-BCF7-4FF8-A082-3F18C7DAEBC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F279A84-27A3-408A-9E90-41023FCCA547}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" xr2:uid="{63A3425B-6033-479B-8BF1-9D375DE2499F}"/>
   </bookViews>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A814EA-F008-428D-8D17-C9F98DC7D045}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="B33" zoomScale="199" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1057,29 +1057,33 @@
     <row r="35" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B35" s="17"/>
       <c r="C35" s="11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E35" s="7"/>
+      <c r="E35" s="7">
+        <v>3</v>
+      </c>
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B36" s="17"/>
       <c r="C36" s="11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E36" s="7"/>
+      <c r="E36" s="7">
+        <v>3</v>
+      </c>
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B37" s="17"/>
       <c r="C37" s="11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>10</v>
@@ -1092,7 +1096,7 @@
     <row r="38" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B38" s="17"/>
       <c r="C38" s="11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>29</v>
@@ -1105,7 +1109,7 @@
     <row r="39" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B39" s="17"/>
       <c r="C39" s="11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>11</v>
@@ -1118,7 +1122,7 @@
     <row r="40" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B40" s="17"/>
       <c r="C40" s="11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>18</v>
@@ -1131,7 +1135,7 @@
     <row r="41" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B41" s="17"/>
       <c r="C41" s="11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>12</v>
@@ -1144,7 +1148,7 @@
     <row r="42" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B42" s="17"/>
       <c r="C42" s="11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>13</v>
@@ -1157,7 +1161,7 @@
     <row r="43" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B43" s="17"/>
       <c r="C43" s="11">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>14</v>
@@ -1170,7 +1174,7 @@
     <row r="44" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B44" s="17"/>
       <c r="C44" s="11">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>43</v>
@@ -1298,7 +1302,7 @@
       </c>
       <c r="E55">
         <f>SUM(E4:E51)</f>
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>